<commit_message>
Add telephone prefix number for provinces
</commit_message>
<xml_diff>
--- a/xlsx/provinces.xlsx
+++ b/xlsx/provinces.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\My Github repositories\iran cities and provinces\list-of-cities-in-Iran\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C27C9B-04CC-4DE0-AD77-FC423BB1FC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-25335" yWindow="2685" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="provinces" sheetId="1" r:id="rId2"/>
+    <sheet name="provinces" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>id</t>
   </si>
@@ -139,16 +146,117 @@
   </si>
   <si>
     <t>یزد</t>
+  </si>
+  <si>
+    <t>tel_prefix</t>
+  </si>
+  <si>
+    <t>041</t>
+  </si>
+  <si>
+    <t>044</t>
+  </si>
+  <si>
+    <t>045</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>084</t>
+  </si>
+  <si>
+    <t>077</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>038</t>
+  </si>
+  <si>
+    <t>056</t>
+  </si>
+  <si>
+    <t>051</t>
+  </si>
+  <si>
+    <t>058</t>
+  </si>
+  <si>
+    <t>061</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>054</t>
+  </si>
+  <si>
+    <t>071</t>
+  </si>
+  <si>
+    <t>028</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>087</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
+    <t>083</t>
+  </si>
+  <si>
+    <t>074</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>066</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>086</t>
+  </si>
+  <si>
+    <t>076</t>
+  </si>
+  <si>
+    <t>081</t>
+  </si>
+  <si>
+    <t>035</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,21 +279,336 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -195,8 +618,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -206,8 +632,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -217,8 +646,11 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="D3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -228,8 +660,11 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -239,8 +674,11 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -250,8 +688,11 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -261,8 +702,11 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -272,8 +716,11 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -283,8 +730,11 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="D9" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -294,8 +744,11 @@
       <c r="C10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -305,8 +758,11 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="D11" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -316,8 +772,11 @@
       <c r="C12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="D12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -327,8 +786,11 @@
       <c r="C13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -338,8 +800,11 @@
       <c r="C14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="D14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -349,8 +814,11 @@
       <c r="C15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="D15" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -360,8 +828,11 @@
       <c r="C16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17">
+      <c r="D16" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -371,8 +842,11 @@
       <c r="C17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18">
+      <c r="D17" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -382,8 +856,11 @@
       <c r="C18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="D18" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -393,8 +870,11 @@
       <c r="C19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="D19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -404,8 +884,11 @@
       <c r="C20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21">
+      <c r="D20" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -415,8 +898,11 @@
       <c r="C21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22">
+      <c r="D21" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -426,8 +912,11 @@
       <c r="C22" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="D22" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -437,8 +926,11 @@
       <c r="C23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24">
+      <c r="D23" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -448,8 +940,11 @@
       <c r="C24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25">
+      <c r="D24" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -459,8 +954,11 @@
       <c r="C25" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26">
+      <c r="D25" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -470,8 +968,11 @@
       <c r="C26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27">
+      <c r="D26" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -481,8 +982,11 @@
       <c r="C27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28">
+      <c r="D27" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -492,8 +996,11 @@
       <c r="C28" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="D28" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -503,8 +1010,11 @@
       <c r="C29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30">
+      <c r="D29" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -514,8 +1024,11 @@
       <c r="C30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31">
+      <c r="D30" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -525,8 +1038,11 @@
       <c r="C31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32">
+      <c r="D31" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -536,7 +1052,11 @@
       <c r="C32" t="s">
         <v>41</v>
       </c>
+      <c r="D32" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add telephone prefix number for provinces (#39)
* Add telephone prefix number for provinces

* Update provinces.txt

* Update CityProvinceQuery.py

* Update README.md

---------

Co-authored-by: Sajad Dehshiri <sajaddp71@gmail.com>
</commit_message>
<xml_diff>
--- a/xlsx/provinces.xlsx
+++ b/xlsx/provinces.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\My Github repositories\iran cities and provinces\list-of-cities-in-Iran\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C27C9B-04CC-4DE0-AD77-FC423BB1FC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-25335" yWindow="2685" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="provinces" sheetId="1" r:id="rId2"/>
+    <sheet name="provinces" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>id</t>
   </si>
@@ -139,16 +146,117 @@
   </si>
   <si>
     <t>یزد</t>
+  </si>
+  <si>
+    <t>tel_prefix</t>
+  </si>
+  <si>
+    <t>041</t>
+  </si>
+  <si>
+    <t>044</t>
+  </si>
+  <si>
+    <t>045</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>084</t>
+  </si>
+  <si>
+    <t>077</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>038</t>
+  </si>
+  <si>
+    <t>056</t>
+  </si>
+  <si>
+    <t>051</t>
+  </si>
+  <si>
+    <t>058</t>
+  </si>
+  <si>
+    <t>061</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>054</t>
+  </si>
+  <si>
+    <t>071</t>
+  </si>
+  <si>
+    <t>028</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>087</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
+    <t>083</t>
+  </si>
+  <si>
+    <t>074</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>066</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>086</t>
+  </si>
+  <si>
+    <t>076</t>
+  </si>
+  <si>
+    <t>081</t>
+  </si>
+  <si>
+    <t>035</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,21 +279,336 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -195,8 +618,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -206,8 +632,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -217,8 +646,11 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="D3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -228,8 +660,11 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -239,8 +674,11 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -250,8 +688,11 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -261,8 +702,11 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -272,8 +716,11 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -283,8 +730,11 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="D9" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -294,8 +744,11 @@
       <c r="C10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -305,8 +758,11 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="D11" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -316,8 +772,11 @@
       <c r="C12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="D12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -327,8 +786,11 @@
       <c r="C13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -338,8 +800,11 @@
       <c r="C14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="D14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -349,8 +814,11 @@
       <c r="C15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="D15" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -360,8 +828,11 @@
       <c r="C16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17">
+      <c r="D16" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -371,8 +842,11 @@
       <c r="C17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18">
+      <c r="D17" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -382,8 +856,11 @@
       <c r="C18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="D18" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -393,8 +870,11 @@
       <c r="C19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="D19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -404,8 +884,11 @@
       <c r="C20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21">
+      <c r="D20" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -415,8 +898,11 @@
       <c r="C21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22">
+      <c r="D21" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -426,8 +912,11 @@
       <c r="C22" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="D22" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -437,8 +926,11 @@
       <c r="C23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24">
+      <c r="D23" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -448,8 +940,11 @@
       <c r="C24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25">
+      <c r="D24" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -459,8 +954,11 @@
       <c r="C25" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26">
+      <c r="D25" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -470,8 +968,11 @@
       <c r="C26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27">
+      <c r="D26" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -481,8 +982,11 @@
       <c r="C27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28">
+      <c r="D27" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -492,8 +996,11 @@
       <c r="C28" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="D28" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -503,8 +1010,11 @@
       <c r="C29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30">
+      <c r="D29" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -514,8 +1024,11 @@
       <c r="C30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31">
+      <c r="D30" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -525,8 +1038,11 @@
       <c r="C31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32">
+      <c r="D31" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -536,7 +1052,11 @@
       <c r="C32" t="s">
         <v>41</v>
       </c>
+      <c r="D32" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>